<commit_message>
refactoring risk analysis. count info now working
</commit_message>
<xml_diff>
--- a/tests/resources/risks.xlsx
+++ b/tests/resources/risks.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q2_20_21 All" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q2_20_21 all data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q2_20_21 Count" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1748,4 +1749,701 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:F47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BRD Risk Category</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Economic</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Technological</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Political</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Legal</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Social</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Environmental</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BRD Primary Risk to</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Schedule</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Benefits</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BRD Internal Control</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Treat - Prevent</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Treat - Directive</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Treat - Corrective</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Tolerate</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BRD Residual Impact</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>5</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Very Low</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BRD Residual Likelihood</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>15</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>8</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Severity Score Risk Category</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>18</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>9</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BRD Has this Risk turned into an Issue?</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>6</v>
+      </c>
+      <c r="D46" t="n">
+        <v>15</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" t="n">
+        <v>3</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
risk analysis working. ready for user testing
</commit_message>
<xml_diff>
--- a/tests/resources/risks.xlsx
+++ b/tests/resources/risks.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q2_20_21 all data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q2_20_21 Count" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q1_20_21 all data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q1_20_21 Count" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -367,7 +367,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brief Risk Decription </t>
+          <t xml:space="preserve">Brief Risk Description </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1859,13 +1859,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -1981,13 +1981,13 @@
         <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -2027,13 +2027,13 @@
         <v>5</v>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -2149,13 +2149,13 @@
         <v>3</v>
       </c>
       <c r="D27" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28">
@@ -2252,13 +2252,13 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
@@ -2336,13 +2336,13 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41">
@@ -2420,13 +2420,13 @@
         <v>6</v>
       </c>
       <c r="D46" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47">

</xml_diff>

<commit_message>
risks class refactored to latest data structure"
</commit_message>
<xml_diff>
--- a/tests/resources/risks.xlsx
+++ b/tests/resources/risks.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:L21"/>
+  <dimension ref="A3:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -357,6 +357,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DfT Group</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Project Name</t>
@@ -414,6 +419,11 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -466,6 +476,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -518,6 +533,11 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -570,6 +590,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -622,6 +647,11 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -674,6 +704,11 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -726,6 +761,11 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -778,6 +818,11 @@
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -830,6 +875,11 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -882,6 +932,11 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -934,6 +989,11 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -986,6 +1046,11 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -1003,6 +1068,11 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -1055,6 +1125,11 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -1087,6 +1162,11 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -1104,6 +1184,11 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -1121,6 +1206,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -1138,6 +1228,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -1753,7 +1848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:L21"/>
+  <dimension ref="A3:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1762,6 +1857,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DfT Group</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Project Name</t>
@@ -1819,6 +1919,11 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -1871,6 +1976,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -1923,6 +2033,11 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -1975,6 +2090,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -2027,6 +2147,11 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -2079,6 +2204,11 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Mars</t>
@@ -2131,6 +2261,11 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -2183,6 +2318,11 @@
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -2235,6 +2375,11 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -2287,6 +2432,11 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -2339,6 +2489,11 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -2391,6 +2546,11 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>SoT</t>
@@ -2408,6 +2568,11 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -2460,6 +2625,11 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -2492,6 +2662,11 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -2509,6 +2684,11 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -2526,6 +2706,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>Columbia</t>
@@ -2543,6 +2728,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Rail</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>Columbia</t>

</xml_diff>